<commit_message>
Update SRH group data
</commit_message>
<xml_diff>
--- a/data/srh_group_data.xlsx
+++ b/data/srh_group_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13860"/>
+    <workbookView xWindow="1380" yWindow="1580" windowWidth="25600" windowHeight="13860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="41">
   <si>
     <t>height</t>
   </si>
@@ -98,9 +95,6 @@
     <t>brown</t>
   </si>
   <si>
-    <t>Shoesize</t>
-  </si>
-  <si>
     <t>Dorthe</t>
   </si>
   <si>
@@ -132,6 +126,27 @@
   </si>
   <si>
     <t>darkbrown</t>
+  </si>
+  <si>
+    <t>Sine</t>
+  </si>
+  <si>
+    <t>Julien</t>
+  </si>
+  <si>
+    <t>shoe size</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>Nana</t>
+  </si>
+  <si>
+    <t>grey</t>
   </si>
 </sst>
 </file>
@@ -483,368 +498,476 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>162</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2">
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>179</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4">
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>164</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6">
+        <v>39</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>175</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E7">
         <v>39</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>178</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E8">
         <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>172</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E9">
         <v>39</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>163</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E10">
         <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>167</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <v>41</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>166</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E12">
         <v>39</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>178</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13">
         <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>195</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14">
         <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>174</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E15">
         <v>37</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>183</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16">
+        <v>41</v>
       </c>
       <c r="F16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>169</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E17">
         <v>38</v>
       </c>
       <c r="F17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>185</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E18">
         <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B19">
         <v>200</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E19">
         <v>50</v>
       </c>
       <c r="F19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20">
         <v>182</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E20">
         <v>45</v>
       </c>
       <c r="F20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B21">
         <v>164</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E21">
         <v>37</v>
       </c>
       <c r="F21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B22">
         <v>184</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E22">
         <v>42</v>
       </c>
       <c r="F22" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <v>175</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>40</v>
+      </c>
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <v>185</v>
+      </c>
+      <c r="D24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>45</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25">
+        <v>182</v>
+      </c>
+      <c r="D25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25">
+        <v>41</v>
+      </c>
+      <c r="F25" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>